<commit_message>
update laporan dan fix halaman
</commit_message>
<xml_diff>
--- a/upload/laporanUraianComplainDivisi.xlsx
+++ b/upload/laporanUraianComplainDivisi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -48,90 +48,6 @@
   </si>
   <si>
     <t>Tanggal</t>
-  </si>
-  <si>
-    <t>ZN23000497</t>
-  </si>
-  <si>
-    <t>ZM23000515</t>
-  </si>
-  <si>
-    <t>009450</t>
-  </si>
-  <si>
-    <t>FC</t>
-  </si>
-  <si>
-    <t>FC0N</t>
-  </si>
-  <si>
-    <t>PRINTER THERMAL TIDAK BISA BUKA</t>
-  </si>
-  <si>
-    <t>03-FEB-23 14:18</t>
-  </si>
-  <si>
-    <t>batal</t>
-  </si>
-  <si>
-    <t>03-FEB-23</t>
-  </si>
-  <si>
-    <t>ZN23000468</t>
-  </si>
-  <si>
-    <t>ZM23000495</t>
-  </si>
-  <si>
-    <t>008127</t>
-  </si>
-  <si>
-    <t>NB7R</t>
-  </si>
-  <si>
-    <t>AGV-SERVER-STATION TIDAK KONEK JARINGAN</t>
-  </si>
-  <si>
-    <t>03-FEB-23 08:26</t>
-  </si>
-  <si>
-    <t>ZN23000492</t>
-  </si>
-  <si>
-    <t>ZM23000517</t>
-  </si>
-  <si>
-    <t>012646</t>
-  </si>
-  <si>
-    <t>FC06</t>
-  </si>
-  <si>
-    <t>TIDAK MUNCUL FILE MENU DI DESKTOP</t>
-  </si>
-  <si>
-    <t>04-FEB-23 14:38</t>
-  </si>
-  <si>
-    <t>04-FEB-23</t>
-  </si>
-  <si>
-    <t>ZN23000449</t>
-  </si>
-  <si>
-    <t>ZM23000476</t>
-  </si>
-  <si>
-    <t>FC13</t>
-  </si>
-  <si>
-    <t>GOOGLE CHROME LEMOT</t>
-  </si>
-  <si>
-    <t>02-FEB-23 09:07</t>
-  </si>
-  <si>
-    <t>02-FEB-23</t>
   </si>
 </sst>
 </file>
@@ -471,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,146 +428,6 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>